<commit_message>
Cleaned up files, ran timing experiments
</commit_message>
<xml_diff>
--- a/lab5/expOutput.xlsx
+++ b/lab5/expOutput.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\CS423\lab5\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985"/>
   </bookViews>
   <sheets>
     <sheet name="expOutput" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -586,41 +581,29 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Alignments Scores for Different Sequence Sizes</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -636,19 +619,76 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:val>
+          <c:xVal>
+            <c:numRef>
+              <c:f>expOutput!$A$2:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>expOutput!$B$2:$B$20</c:f>
               <c:numCache>
@@ -713,7 +753,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
@@ -730,19 +770,76 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:val>
+          <c:xVal>
+            <c:numRef>
+              <c:f>expOutput!$A$2:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>expOutput!$C$2:$C$20</c:f>
               <c:numCache>
@@ -807,7 +904,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
@@ -818,185 +915,92 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="533016880"/>
-        <c:axId val="533014528"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="533016880"/>
+        <c:axId val="168421248"/>
+        <c:axId val="168419712"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="168421248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="95"/>
+          <c:min val="5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorTickMark val="none"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Sequence Size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="533014528"/>
+        <c:crossAx val="168419712"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="15"/>
+        <c:minorUnit val="5"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="533014528"/>
+        <c:axId val="168419712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Alignment Score</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="533016880"/>
+        <c:crossAx val="168421248"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -1005,580 +1009,24 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>38099</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>61911</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1639,7 +1087,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1674,7 +1122,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1851,7 +1299,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1862,10 +1310,15 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T30" sqref="T30"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>